<commit_message>
Minor fix to component counts and added component emissions tables
</commit_message>
<xml_diff>
--- a/2_Methane_Database/Table_Comp_Counts.xlsx
+++ b/2_Methane_Database/Table_Comp_Counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ru3\Dropbox\Doctoral\Projects\Research Projects\manuscripts\2_BU_paper\3_Analysis\3_Methane_Database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ru3\Dropbox\Doctoral\Projects\Research Projects\manuscripts\2_BU_paper\3_Analysis\2_Methane_Database\FINAL POST REVISION VERSIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CACF900-2838-4DD6-8D86-F7A274F79728}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AD43004-5E7C-492A-AF4C-052B6A542C50}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3324" yWindow="0" windowWidth="13200" windowHeight="9396" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Counts_Table" sheetId="2" r:id="rId1"/>
@@ -656,21 +656,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A892F7B8-E706-48A0-A3B1-81AAFAD658D3}">
   <dimension ref="C5:P24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="3:16" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:16" ht="46" x14ac:dyDescent="0.35">
       <c r="C7" s="8"/>
       <c r="D7" s="7" t="s">
         <v>17</v>
@@ -710,21 +710,21 @@
       </c>
       <c r="P7" s="2"/>
     </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C8" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D8" s="2" t="str">
         <f>Counts_Data!O30&amp;"-"&amp;Counts_Data!O64</f>
-        <v>74-298</v>
+        <v>69-298</v>
       </c>
       <c r="E8" s="2" t="str">
         <f>Counts_Data!P30&amp;"-"&amp;Counts_Data!P64</f>
-        <v>13-27</v>
+        <v>12-23</v>
       </c>
       <c r="F8" s="2" t="str">
         <f>Counts_Data!Q30&amp;"-"&amp;Counts_Data!Q64</f>
-        <v>1-5</v>
+        <v>1-3</v>
       </c>
       <c r="G8" s="2" t="str">
         <f>Counts_Data!R30&amp;"-"&amp;Counts_Data!R64</f>
@@ -758,29 +758,29 @@
       </c>
       <c r="P8" s="2"/>
     </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C9" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D9" s="2" t="str">
         <f>Counts_Data!O32&amp;"-"&amp;Counts_Data!O66</f>
-        <v>20-177</v>
+        <v>20-117</v>
       </c>
       <c r="E9" s="2" t="str">
         <f>Counts_Data!P32&amp;"-"&amp;Counts_Data!P66</f>
-        <v>2-29</v>
+        <v>2-19</v>
       </c>
       <c r="F9" s="2" t="str">
         <f>Counts_Data!Q32&amp;"-"&amp;Counts_Data!Q66</f>
-        <v>1-5</v>
+        <v>1-3</v>
       </c>
       <c r="G9" s="2" t="str">
         <f>Counts_Data!R32&amp;"-"&amp;Counts_Data!R66</f>
-        <v>1-2</v>
+        <v>1-1</v>
       </c>
       <c r="H9" s="2" t="str">
         <f>Counts_Data!S32&amp;"-"&amp;Counts_Data!S66</f>
-        <v>1-1</v>
+        <v>0-0</v>
       </c>
       <c r="I9" s="2" t="str">
         <f>Counts_Data!T32&amp;"-"&amp;Counts_Data!T66</f>
@@ -807,21 +807,21 @@
       </c>
       <c r="P9" s="2"/>
     </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C10" s="5" t="s">
         <v>3</v>
       </c>
       <c r="D10" s="2" t="str">
         <f>Counts_Data!O33&amp;"-"&amp;Counts_Data!O67</f>
-        <v>62-125</v>
+        <v>62-180</v>
       </c>
       <c r="E10" s="2" t="str">
         <f>Counts_Data!P33&amp;"-"&amp;Counts_Data!P67</f>
-        <v>12-28</v>
+        <v>20-29</v>
       </c>
       <c r="F10" s="2" t="str">
         <f>Counts_Data!Q33&amp;"-"&amp;Counts_Data!Q67</f>
-        <v>1-1</v>
+        <v>1-5</v>
       </c>
       <c r="G10" s="2" t="str">
         <f>Counts_Data!R33&amp;"-"&amp;Counts_Data!R67</f>
@@ -855,7 +855,7 @@
       </c>
       <c r="P10" s="2"/>
     </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C11" s="5" t="s">
         <v>20</v>
       </c>
@@ -903,29 +903,29 @@
       </c>
       <c r="P11" s="2"/>
     </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
       <c r="D12" s="2" t="str">
         <f>Counts_Data!O35&amp;"-"&amp;Counts_Data!O69</f>
-        <v>3-179</v>
+        <v>3-54</v>
       </c>
       <c r="E12" s="2" t="str">
         <f>Counts_Data!P35&amp;"-"&amp;Counts_Data!P69</f>
-        <v>1-31</v>
+        <v>1-7</v>
       </c>
       <c r="F12" s="2" t="str">
         <f>Counts_Data!Q35&amp;"-"&amp;Counts_Data!Q69</f>
-        <v>1-9</v>
+        <v>1-2</v>
       </c>
       <c r="G12" s="2" t="str">
         <f>Counts_Data!R35&amp;"-"&amp;Counts_Data!R69</f>
-        <v>1-14</v>
+        <v>1-1</v>
       </c>
       <c r="H12" s="2" t="str">
         <f>Counts_Data!S35&amp;"-"&amp;Counts_Data!S69</f>
-        <v>2-2</v>
+        <v>0-0</v>
       </c>
       <c r="I12" s="2" t="str">
         <f>Counts_Data!T35&amp;"-"&amp;Counts_Data!T69</f>
@@ -951,13 +951,13 @@
       </c>
       <c r="P12" s="2"/>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C13" s="5" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="2" t="str">
         <f>Counts_Data!O37&amp;"-"&amp;Counts_Data!O71</f>
-        <v>120-586</v>
+        <v>226-586</v>
       </c>
       <c r="E13" s="2" t="str">
         <f>Counts_Data!P37&amp;"-"&amp;Counts_Data!P71</f>
@@ -965,15 +965,15 @@
       </c>
       <c r="F13" s="2" t="str">
         <f>Counts_Data!Q37&amp;"-"&amp;Counts_Data!Q71</f>
-        <v>1-4</v>
+        <v>1-5</v>
       </c>
       <c r="G13" s="2" t="str">
         <f>Counts_Data!R37&amp;"-"&amp;Counts_Data!R71</f>
-        <v>1-4</v>
+        <v>2-4</v>
       </c>
       <c r="H13" s="2" t="str">
         <f>Counts_Data!S37&amp;"-"&amp;Counts_Data!S71</f>
-        <v>4-4</v>
+        <v>2-4</v>
       </c>
       <c r="I13" s="2" t="str">
         <f>Counts_Data!T37&amp;"-"&amp;Counts_Data!T71</f>
@@ -1000,7 +1000,7 @@
       </c>
       <c r="P13" s="2"/>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1014,7 +1014,7 @@
       </c>
       <c r="F14" s="2" t="str">
         <f>Counts_Data!Q38&amp;"-"&amp;Counts_Data!Q72</f>
-        <v>1-1</v>
+        <v>1-5</v>
       </c>
       <c r="G14" s="2" t="str">
         <f>Counts_Data!R38&amp;"-"&amp;Counts_Data!R72</f>
@@ -1022,7 +1022,7 @@
       </c>
       <c r="H14" s="2" t="str">
         <f>Counts_Data!S38&amp;"-"&amp;Counts_Data!S72</f>
-        <v>0-0</v>
+        <v>1-1</v>
       </c>
       <c r="I14" s="2" t="str">
         <f>Counts_Data!T38&amp;"-"&amp;Counts_Data!T72</f>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="P14" s="2"/>
     </row>
-    <row r="15" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C15" s="5" t="s">
         <v>1</v>
       </c>
@@ -1074,9 +1074,8 @@
       <c r="J15" s="2">
         <v>0</v>
       </c>
-      <c r="K15" s="2" t="str">
-        <f>Counts_Data!V39&amp;"-"&amp;Counts_Data!V73</f>
-        <v>1-1</v>
+      <c r="K15" s="2">
+        <v>1</v>
       </c>
       <c r="L15" s="2">
         <v>0</v>
@@ -1092,7 +1091,7 @@
       </c>
       <c r="P15" s="2"/>
     </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C16" s="4" t="s">
         <v>0</v>
       </c>
@@ -1114,9 +1113,8 @@
       <c r="I16" s="3">
         <v>0</v>
       </c>
-      <c r="J16" s="3" t="str">
-        <f>Counts_Data!U40&amp;"-"&amp;Counts_Data!U74</f>
-        <v>1-1</v>
+      <c r="J16" s="3">
+        <v>1</v>
       </c>
       <c r="K16" s="3">
         <v>0</v>
@@ -1135,7 +1133,7 @@
       </c>
       <c r="P16" s="2"/>
     </row>
-    <row r="18" spans="3:16" ht="46.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:16" ht="46" x14ac:dyDescent="0.35">
       <c r="C18" s="8"/>
       <c r="D18" s="7" t="s">
         <v>17</v>
@@ -1175,7 +1173,7 @@
       </c>
       <c r="P18" s="2"/>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C19" s="6" t="s">
         <v>5</v>
       </c>
@@ -1221,7 +1219,7 @@
       </c>
       <c r="P19" s="2"/>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="20" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C20" s="5" t="s">
         <v>4</v>
       </c>
@@ -1268,7 +1266,7 @@
       </c>
       <c r="P20" s="2"/>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="21" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C21" s="5" t="s">
         <v>3</v>
       </c>
@@ -1315,7 +1313,7 @@
       </c>
       <c r="P21" s="2"/>
     </row>
-    <row r="22" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="22" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C22" s="5" t="s">
         <v>2</v>
       </c>
@@ -1363,7 +1361,7 @@
       </c>
       <c r="P22" s="2"/>
     </row>
-    <row r="23" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="23" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C23" s="5" t="s">
         <v>1</v>
       </c>
@@ -1388,9 +1386,8 @@
       <c r="J23" s="2">
         <v>0</v>
       </c>
-      <c r="K23" s="2" t="str">
-        <f>CONCATENATE(Counts_Data!V22&amp;"-"&amp;Counts_Data!V56)</f>
-        <v>1-1</v>
+      <c r="K23" s="2">
+        <v>1</v>
       </c>
       <c r="L23" s="2">
         <v>0</v>
@@ -1406,7 +1403,7 @@
       </c>
       <c r="P23" s="2"/>
     </row>
-    <row r="24" spans="3:16" x14ac:dyDescent="0.3">
+    <row r="24" spans="3:16" x14ac:dyDescent="0.35">
       <c r="C24" s="4" t="s">
         <v>0</v>
       </c>
@@ -1428,9 +1425,8 @@
       <c r="I24" s="3">
         <v>0</v>
       </c>
-      <c r="J24" s="3" t="str">
-        <f>CONCATENATE(Counts_Data!U23&amp;"-"&amp;Counts_Data!U57)</f>
-        <v>1-1</v>
+      <c r="J24" s="3">
+        <v>1</v>
       </c>
       <c r="K24" s="3">
         <v>0</v>
@@ -1458,54 +1454,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C16A8BA-0453-4E8D-89BF-AEE5D7F27D34}">
   <dimension ref="A3:Z93"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
       <selection activeCell="J28" sqref="J28"/>
-      <selection pane="topRight" activeCell="Q14" sqref="Q14"/>
+      <selection pane="topRight" activeCell="O64" sqref="O64:Z74"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.77734375" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="9.21875" style="1"/>
+    <col min="1" max="1" width="24.81640625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.35">
       <c r="B4" s="1" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C5" s="1" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C6" s="1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C7" s="1" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:26" s="10" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A8" s="11" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.35">
       <c r="N10" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
@@ -1540,7 +1536,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1608,7 +1604,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1622,10 +1618,10 @@
         <v>6.64</v>
       </c>
       <c r="E13" s="1">
-        <v>0.941909</v>
+        <v>0.94190871369294604</v>
       </c>
       <c r="F13" s="1">
-        <v>5.4949999999999999E-3</v>
+        <v>5.4945054945054949E-3</v>
       </c>
       <c r="G13" s="1">
         <v>0</v>
@@ -1649,35 +1645,35 @@
         <v>27</v>
       </c>
       <c r="O13" s="1">
-        <f>ROUNDUP(C13,0)</f>
+        <f t="shared" ref="O13:O23" si="0">ROUNDUP(C13,0)</f>
         <v>61</v>
       </c>
       <c r="P13" s="1">
-        <f>ROUNDUP(D13,0)</f>
+        <f t="shared" ref="P13:P23" si="1">ROUNDUP(D13,0)</f>
         <v>7</v>
       </c>
       <c r="Q13" s="1">
-        <f>ROUNDUP(E13,0)</f>
+        <f t="shared" ref="Q13:Q23" si="2">ROUNDUP(E13,0)</f>
         <v>1</v>
       </c>
       <c r="R13" s="1">
-        <f>ROUNDUP(F13,0)</f>
+        <f t="shared" ref="R13:R23" si="3">ROUNDUP(F13,0)</f>
         <v>1</v>
       </c>
       <c r="S13" s="1">
-        <f>ROUNDUP(G13,0)</f>
+        <f t="shared" ref="S13:S23" si="4">ROUNDUP(G13,0)</f>
         <v>0</v>
       </c>
       <c r="T13" s="1">
-        <f>ROUNDUP(H13,0)</f>
+        <f t="shared" ref="T13:T23" si="5">ROUNDUP(H13,0)</f>
         <v>0</v>
       </c>
       <c r="U13" s="1">
-        <f>ROUNDUP(I13,0)</f>
+        <f t="shared" ref="U13:U23" si="6">ROUNDUP(I13,0)</f>
         <v>0</v>
       </c>
       <c r="V13" s="1">
-        <f>ROUNDUP(J13,0)</f>
+        <f t="shared" ref="V13:V23" si="7">ROUNDUP(J13,0)</f>
         <v>0</v>
       </c>
       <c r="W13" s="1">
@@ -1690,11 +1686,11 @@
         <v>0</v>
       </c>
       <c r="Z13" s="1">
-        <f>ROUNDUP(L13,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Z13:Z23" si="8">ROUNDUP(L13,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -1702,16 +1698,16 @@
         <v>26</v>
       </c>
       <c r="C14" s="1">
-        <v>22.310369999999999</v>
+        <v>22.310370370370372</v>
       </c>
       <c r="D14" s="1">
         <v>1.49</v>
       </c>
       <c r="E14" s="1">
-        <v>0.45588200000000001</v>
+        <v>0.45588235294117646</v>
       </c>
       <c r="F14" s="1">
-        <v>9.5238000000000003E-2</v>
+        <v>9.5238095238095233E-2</v>
       </c>
       <c r="G14" s="1">
         <v>0</v>
@@ -1735,35 +1731,35 @@
         <v>26</v>
       </c>
       <c r="O14" s="1">
-        <f>ROUNDUP(C14,0)</f>
+        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="P14" s="1">
-        <f>ROUNDUP(D14,0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q14" s="1">
-        <f>ROUNDUP(E14,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="R14" s="1">
-        <f>ROUNDUP(F14,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S14" s="1">
-        <f>ROUNDUP(G14,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T14" s="1">
-        <f>ROUNDUP(H14,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U14" s="1">
-        <f>ROUNDUP(I14,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V14" s="1">
-        <f>ROUNDUP(J14,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W14" s="1">
@@ -1776,11 +1772,11 @@
         <v>0</v>
       </c>
       <c r="Z14" s="1">
-        <f>ROUNDUP(L14,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>21</v>
       </c>
@@ -1788,16 +1784,16 @@
         <v>25</v>
       </c>
       <c r="C15" s="1">
-        <v>29.309550000000002</v>
+        <v>29.309545454545454</v>
       </c>
       <c r="D15" s="1">
         <v>2.52</v>
       </c>
       <c r="E15" s="1">
-        <v>0.82954499999999998</v>
+        <v>0.82954545454545459</v>
       </c>
       <c r="F15" s="1">
-        <v>0.212121</v>
+        <v>0.21212121212121213</v>
       </c>
       <c r="G15" s="1">
         <v>0</v>
@@ -1821,35 +1817,35 @@
         <v>25</v>
       </c>
       <c r="O15" s="1">
-        <f>ROUNDUP(C15,0)</f>
+        <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="P15" s="1">
-        <f>ROUNDUP(D15,0)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="Q15" s="1">
-        <f>ROUNDUP(E15,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="R15" s="1">
-        <f>ROUNDUP(F15,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S15" s="1">
-        <f>ROUNDUP(G15,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T15" s="1">
-        <f>ROUNDUP(H15,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U15" s="1">
-        <f>ROUNDUP(I15,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V15" s="1">
-        <f>ROUNDUP(J15,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W15" s="1">
@@ -1862,11 +1858,11 @@
         <v>0</v>
       </c>
       <c r="Z15" s="1">
-        <f>ROUNDUP(L15,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>3</v>
       </c>
@@ -1907,35 +1903,35 @@
         <v>24</v>
       </c>
       <c r="O16" s="1">
-        <f>ROUNDUP(C16,0)</f>
+        <f t="shared" si="0"/>
         <v>62</v>
       </c>
       <c r="P16" s="1">
-        <f>ROUNDUP(D16,0)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="Q16" s="1">
-        <f>ROUNDUP(E16,0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R16" s="1">
-        <f>ROUNDUP(F16,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S16" s="1">
-        <f>ROUNDUP(G16,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T16" s="1">
-        <f>ROUNDUP(H16,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U16" s="1">
-        <f>ROUNDUP(I16,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V16" s="1">
-        <f>ROUNDUP(J16,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W16" s="1">
@@ -1948,11 +1944,11 @@
         <v>0</v>
       </c>
       <c r="Z16" s="1">
-        <f>ROUNDUP(L16,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1960,13 +1956,13 @@
         <v>23</v>
       </c>
       <c r="C17" s="1">
-        <v>13.44</v>
+        <v>13.440000000000001</v>
       </c>
       <c r="D17" s="1">
         <v>0.85</v>
       </c>
       <c r="E17" s="1">
-        <v>1.9166669999999999</v>
+        <v>1.9166666666666667</v>
       </c>
       <c r="F17" s="1">
         <v>0.25</v>
@@ -1993,35 +1989,35 @@
         <v>23</v>
       </c>
       <c r="O17" s="1">
-        <f>ROUNDUP(C17,0)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="P17" s="1">
-        <f>ROUNDUP(D17,0)</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="Q17" s="1">
-        <f>ROUNDUP(E17,0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R17" s="1">
-        <f>ROUNDUP(F17,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S17" s="1">
-        <f>ROUNDUP(G17,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T17" s="1">
-        <f>ROUNDUP(H17,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U17" s="1">
-        <f>ROUNDUP(I17,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V17" s="1">
-        <f>ROUNDUP(J17,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W17" s="1">
@@ -2034,11 +2030,11 @@
         <v>0</v>
       </c>
       <c r="Z17" s="1">
-        <f>ROUNDUP(L17,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -2055,10 +2051,10 @@
         <v>0.01</v>
       </c>
       <c r="F18" s="1">
-        <v>8.3333000000000004E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G18" s="1">
-        <v>4.1667000000000003E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H18" s="1">
         <v>1</v>
@@ -2079,35 +2075,35 @@
         <v>44</v>
       </c>
       <c r="O18" s="1">
-        <f>ROUNDUP(C18,0)</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="P18" s="1">
-        <f>ROUNDUP(D18,0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q18" s="1">
-        <f>ROUNDUP(E18,0)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="R18" s="1">
-        <f>ROUNDUP(F18,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S18" s="1">
-        <f>ROUNDUP(G18,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T18" s="1">
-        <f>ROUNDUP(H18,0)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="U18" s="1">
-        <f>ROUNDUP(I18,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V18" s="1">
-        <f>ROUNDUP(J18,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W18" s="1">
@@ -2120,11 +2116,11 @@
         <v>0</v>
       </c>
       <c r="Z18" s="1">
-        <f>ROUNDUP(L18,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>43</v>
       </c>
@@ -2165,35 +2161,35 @@
         <v>42</v>
       </c>
       <c r="O19" s="1">
-        <f>ROUNDUP(C19,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P19" s="1">
-        <f>ROUNDUP(D19,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q19" s="1">
-        <f>ROUNDUP(E19,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R19" s="1">
-        <f>ROUNDUP(F19,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S19" s="1">
-        <f>ROUNDUP(G19,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T19" s="1">
-        <f>ROUNDUP(H19,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U19" s="1">
-        <f>ROUNDUP(I19,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V19" s="1">
-        <f>ROUNDUP(J19,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W19" s="1">
@@ -2206,11 +2202,11 @@
         <v>0</v>
       </c>
       <c r="Z19" s="1">
-        <f>ROUNDUP(L19,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>41</v>
       </c>
@@ -2224,10 +2220,10 @@
         <v>6.06</v>
       </c>
       <c r="E20" s="1">
-        <v>1.8333330000000001</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="F20" s="1">
-        <v>0.16666700000000001</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G20" s="1">
         <v>1</v>
@@ -2251,35 +2247,35 @@
         <v>40</v>
       </c>
       <c r="O20" s="1">
-        <f>ROUNDUP(C20,0)</f>
+        <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="P20" s="1">
-        <f>ROUNDUP(D20,0)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="Q20" s="1">
-        <f>ROUNDUP(E20,0)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="R20" s="1">
-        <f>ROUNDUP(F20,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S20" s="1">
-        <f>ROUNDUP(G20,0)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="T20" s="1">
-        <f>ROUNDUP(H20,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U20" s="1">
-        <f>ROUNDUP(I20,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V20" s="1">
-        <f>ROUNDUP(J20,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W20" s="1">
@@ -2292,11 +2288,11 @@
         <v>0</v>
       </c>
       <c r="Z20" s="1">
-        <f>ROUNDUP(L20,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>18</v>
       </c>
@@ -2304,7 +2300,7 @@
         <v>39</v>
       </c>
       <c r="C21" s="1">
-        <v>21.56</v>
+        <v>21.560000000000002</v>
       </c>
       <c r="D21" s="1">
         <v>1.45</v>
@@ -2337,35 +2333,35 @@
         <v>39</v>
       </c>
       <c r="O21" s="1">
-        <f>ROUNDUP(C21,0)</f>
+        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="P21" s="1">
-        <f>ROUNDUP(D21,0)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="Q21" s="1">
-        <f>ROUNDUP(E21,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R21" s="1">
-        <f>ROUNDUP(F21,0)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="S21" s="1">
-        <f>ROUNDUP(G21,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T21" s="1">
-        <f>ROUNDUP(H21,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U21" s="1">
-        <f>ROUNDUP(I21,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V21" s="1">
-        <f>ROUNDUP(J21,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W21" s="1">
@@ -2378,11 +2374,11 @@
         <v>0</v>
       </c>
       <c r="Z21" s="1">
-        <f>ROUNDUP(L21,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>38</v>
       </c>
@@ -2423,35 +2419,35 @@
         <v>37</v>
       </c>
       <c r="O22" s="1">
-        <f>ROUNDUP(C22,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P22" s="1">
-        <f>ROUNDUP(D22,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q22" s="1">
-        <f>ROUNDUP(E22,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R22" s="1">
-        <f>ROUNDUP(F22,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S22" s="1">
-        <f>ROUNDUP(G22,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T22" s="1">
-        <f>ROUNDUP(H22,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U22" s="1">
-        <f>ROUNDUP(I22,0)</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="V22" s="1">
-        <f>ROUNDUP(J22,0)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="W22" s="1">
@@ -2464,11 +2460,11 @@
         <v>0</v>
       </c>
       <c r="Z22" s="1">
-        <f>ROUNDUP(L22,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>36</v>
       </c>
@@ -2509,35 +2505,35 @@
         <v>35</v>
       </c>
       <c r="O23" s="1">
-        <f>ROUNDUP(C23,0)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="P23" s="1">
-        <f>ROUNDUP(D23,0)</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q23" s="1">
-        <f>ROUNDUP(E23,0)</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="R23" s="1">
-        <f>ROUNDUP(F23,0)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="S23" s="1">
-        <f>ROUNDUP(G23,0)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="T23" s="1">
-        <f>ROUNDUP(H23,0)</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="U23" s="1">
-        <f>ROUNDUP(I23,0)</f>
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
       <c r="V23" s="1">
-        <f>ROUNDUP(J23,0)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="W23" s="1">
@@ -2550,11 +2546,11 @@
         <v>0</v>
       </c>
       <c r="Z23" s="1">
-        <f>ROUNDUP(L23,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -2619,7 +2615,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C29" s="1" t="s">
         <v>32</v>
       </c>
@@ -2687,7 +2683,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>28</v>
       </c>
@@ -2695,10 +2691,10 @@
         <v>27</v>
       </c>
       <c r="C30" s="1">
-        <v>73.08</v>
+        <v>68.879518072289159</v>
       </c>
       <c r="D30" s="1">
-        <v>12.04</v>
+        <v>11.072289156626505</v>
       </c>
       <c r="E30" s="1">
         <v>0.01</v>
@@ -2707,7 +2703,7 @@
         <v>0.05</v>
       </c>
       <c r="G30" s="1">
-        <v>0</v>
+        <v>1.2048192771084338E-2</v>
       </c>
       <c r="H30" s="1">
         <v>0.39</v>
@@ -2728,35 +2724,35 @@
         <v>27</v>
       </c>
       <c r="O30" s="1">
-        <f>ROUNDUP(C30,0)</f>
-        <v>74</v>
+        <f t="shared" ref="O30:O40" si="9">ROUNDUP(C30,0)</f>
+        <v>69</v>
       </c>
       <c r="P30" s="1">
-        <f>ROUNDUP(D30,0)</f>
-        <v>13</v>
+        <f t="shared" ref="P30:P40" si="10">ROUNDUP(D30,0)</f>
+        <v>12</v>
       </c>
       <c r="Q30" s="1">
-        <f>ROUNDUP(E30,0)</f>
+        <f t="shared" ref="Q30:Q40" si="11">ROUNDUP(E30,0)</f>
         <v>1</v>
       </c>
       <c r="R30" s="1">
-        <f>ROUNDUP(F30,0)</f>
+        <f t="shared" ref="R30:R40" si="12">ROUNDUP(F30,0)</f>
         <v>1</v>
       </c>
       <c r="S30" s="1">
-        <f>ROUNDUP(G30,0)</f>
-        <v>0</v>
+        <f t="shared" ref="S30:S40" si="13">ROUNDUP(G30,0)</f>
+        <v>1</v>
       </c>
       <c r="T30" s="1">
-        <f>ROUNDUP(H30,0)</f>
+        <f t="shared" ref="T30:T40" si="14">ROUNDUP(H30,0)</f>
         <v>1</v>
       </c>
       <c r="U30" s="1">
-        <f>ROUNDUP(I30,0)</f>
+        <f t="shared" ref="U30:U40" si="15">ROUNDUP(I30,0)</f>
         <v>0</v>
       </c>
       <c r="V30" s="1">
-        <f>ROUNDUP(J30,0)</f>
+        <f t="shared" ref="V30:V40" si="16">ROUNDUP(J30,0)</f>
         <v>0</v>
       </c>
       <c r="W30" s="1">
@@ -2769,11 +2765,11 @@
         <v>0</v>
       </c>
       <c r="Z30" s="1">
-        <f>ROUNDUP(L30,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Z30:Z40" si="17">ROUNDUP(L30,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>4</v>
       </c>
@@ -2781,10 +2777,10 @@
         <v>26</v>
       </c>
       <c r="C31" s="1">
-        <v>99.895060000000001</v>
+        <v>99.895061728395063</v>
       </c>
       <c r="D31" s="1">
-        <v>15.438269999999999</v>
+        <v>15.438271604938272</v>
       </c>
       <c r="E31" s="1">
         <v>0.06</v>
@@ -2814,35 +2810,35 @@
         <v>26</v>
       </c>
       <c r="O31" s="1">
-        <f>ROUNDUP(C31,0)</f>
+        <f t="shared" si="9"/>
         <v>100</v>
       </c>
       <c r="P31" s="1">
-        <f>ROUNDUP(D31,0)</f>
+        <f t="shared" si="10"/>
         <v>16</v>
       </c>
       <c r="Q31" s="1">
-        <f>ROUNDUP(E31,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R31" s="1">
-        <f>ROUNDUP(F31,0)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S31" s="1">
-        <f>ROUNDUP(G31,0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T31" s="1">
-        <f>ROUNDUP(H31,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="U31" s="1">
-        <f>ROUNDUP(I31,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V31" s="1">
-        <f>ROUNDUP(J31,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W31" s="1">
@@ -2855,11 +2851,11 @@
         <v>0</v>
       </c>
       <c r="Z31" s="1">
-        <f>ROUNDUP(L31,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>21</v>
       </c>
@@ -2867,19 +2863,19 @@
         <v>25</v>
       </c>
       <c r="C32" s="1">
-        <v>19.239550000000001</v>
+        <v>19.239545454545453</v>
       </c>
       <c r="D32" s="1">
         <v>1.1399999999999999</v>
       </c>
       <c r="E32" s="1">
-        <v>0.82954499999999998</v>
+        <v>0.82954545454545459</v>
       </c>
       <c r="F32" s="1">
-        <v>0.397727</v>
+        <v>0.39772727272727271</v>
       </c>
       <c r="G32" s="1">
-        <v>0.134328</v>
+        <v>0</v>
       </c>
       <c r="H32" s="1">
         <v>1.1100000000000001</v>
@@ -2900,35 +2896,35 @@
         <v>25</v>
       </c>
       <c r="O32" s="1">
-        <f>ROUNDUP(C32,0)</f>
+        <f t="shared" si="9"/>
         <v>20</v>
       </c>
       <c r="P32" s="1">
-        <f>ROUNDUP(D32,0)</f>
+        <f t="shared" si="10"/>
         <v>2</v>
       </c>
       <c r="Q32" s="1">
-        <f>ROUNDUP(E32,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R32" s="1">
-        <f>ROUNDUP(F32,0)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S32" s="1">
-        <f>ROUNDUP(G32,0)</f>
-        <v>1</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="T32" s="1">
-        <f>ROUNDUP(H32,0)</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="U32" s="1">
-        <f>ROUNDUP(I32,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V32" s="1">
-        <f>ROUNDUP(J32,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W32" s="1">
@@ -2941,11 +2937,11 @@
         <v>0</v>
       </c>
       <c r="Z32" s="1">
-        <f>ROUNDUP(L32,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>3</v>
       </c>
@@ -2956,16 +2952,16 @@
         <v>62</v>
       </c>
       <c r="D33" s="1">
-        <v>11.25</v>
+        <v>19.260000000000002</v>
       </c>
       <c r="E33" s="1">
         <v>0.11</v>
       </c>
       <c r="F33" s="1">
-        <v>0.33333299999999999</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="G33" s="1">
-        <v>0</v>
+        <v>0.13432835820895522</v>
       </c>
       <c r="H33" s="1">
         <v>2.39</v>
@@ -2986,35 +2982,35 @@
         <v>24</v>
       </c>
       <c r="O33" s="1">
-        <f>ROUNDUP(C33,0)</f>
+        <f t="shared" si="9"/>
         <v>62</v>
       </c>
       <c r="P33" s="1">
-        <f>ROUNDUP(D33,0)</f>
-        <v>12</v>
+        <f t="shared" si="10"/>
+        <v>20</v>
       </c>
       <c r="Q33" s="1">
-        <f>ROUNDUP(E33,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R33" s="1">
-        <f>ROUNDUP(F33,0)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S33" s="1">
-        <f>ROUNDUP(G33,0)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="T33" s="1">
-        <f>ROUNDUP(H33,0)</f>
+        <f t="shared" si="14"/>
         <v>3</v>
       </c>
       <c r="U33" s="1">
-        <f>ROUNDUP(I33,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V33" s="1">
-        <f>ROUNDUP(J33,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W33" s="1">
@@ -3027,11 +3023,11 @@
         <v>0</v>
       </c>
       <c r="Z33" s="1">
-        <f>ROUNDUP(L33,0)</f>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>20</v>
       </c>
@@ -3072,35 +3068,35 @@
         <v>23</v>
       </c>
       <c r="O34" s="1">
-        <f>ROUNDUP(C34,0)</f>
+        <f t="shared" si="9"/>
         <v>39</v>
       </c>
       <c r="P34" s="1">
-        <f>ROUNDUP(D34,0)</f>
+        <f t="shared" si="10"/>
         <v>3</v>
       </c>
       <c r="Q34" s="1">
-        <f>ROUNDUP(E34,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R34" s="1">
-        <f>ROUNDUP(F34,0)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S34" s="1">
-        <f>ROUNDUP(G34,0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T34" s="1">
-        <f>ROUNDUP(H34,0)</f>
+        <f t="shared" si="14"/>
         <v>2</v>
       </c>
       <c r="U34" s="1">
-        <f>ROUNDUP(I34,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V34" s="1">
-        <f>ROUNDUP(J34,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W34" s="1">
@@ -3113,11 +3109,11 @@
         <v>0</v>
       </c>
       <c r="Z34" s="1">
-        <f>ROUNDUP(L34,0)</f>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>45</v>
       </c>
@@ -3134,10 +3130,10 @@
         <v>0.01</v>
       </c>
       <c r="F35" s="1">
-        <v>0.23</v>
+        <v>8.5714285714285715E-2</v>
       </c>
       <c r="G35" s="1">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="H35" s="1">
         <v>0.23</v>
@@ -3158,35 +3154,35 @@
         <v>44</v>
       </c>
       <c r="O35" s="1">
-        <f>ROUNDUP(C35,0)</f>
+        <f t="shared" si="9"/>
         <v>3</v>
       </c>
       <c r="P35" s="1">
-        <f>ROUNDUP(D35,0)</f>
+        <f t="shared" si="10"/>
         <v>1</v>
       </c>
       <c r="Q35" s="1">
-        <f>ROUNDUP(E35,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R35" s="1">
-        <f>ROUNDUP(F35,0)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S35" s="1">
-        <f>ROUNDUP(G35,0)</f>
-        <v>2</v>
+        <f t="shared" si="13"/>
+        <v>0</v>
       </c>
       <c r="T35" s="1">
-        <f>ROUNDUP(H35,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="U35" s="1">
-        <f>ROUNDUP(I35,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V35" s="1">
-        <f>ROUNDUP(J35,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W35" s="1">
@@ -3199,11 +3195,11 @@
         <v>0</v>
       </c>
       <c r="Z35" s="1">
-        <f>ROUNDUP(L35,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>43</v>
       </c>
@@ -3244,35 +3240,35 @@
         <v>42</v>
       </c>
       <c r="O36" s="1">
-        <f>ROUNDUP(C36,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P36" s="1">
-        <f>ROUNDUP(D36,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q36" s="1">
-        <f>ROUNDUP(E36,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R36" s="1">
-        <f>ROUNDUP(F36,0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S36" s="1">
-        <f>ROUNDUP(G36,0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T36" s="1">
-        <f>ROUNDUP(H36,0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U36" s="1">
-        <f>ROUNDUP(I36,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V36" s="1">
-        <f>ROUNDUP(J36,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W36" s="1">
@@ -3285,11 +3281,11 @@
         <v>0</v>
       </c>
       <c r="Z36" s="1">
-        <f>ROUNDUP(L36,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>41</v>
       </c>
@@ -3297,7 +3293,7 @@
         <v>40</v>
       </c>
       <c r="C37" s="1">
-        <v>119.5</v>
+        <v>225.55555555555554</v>
       </c>
       <c r="D37" s="1">
         <v>17.510000000000002</v>
@@ -3306,10 +3302,10 @@
         <v>0.52</v>
       </c>
       <c r="F37" s="1">
-        <v>1</v>
+        <v>1.8888888888888888</v>
       </c>
       <c r="G37" s="1">
-        <v>3.05</v>
+        <v>1.2777777777777777</v>
       </c>
       <c r="H37" s="1">
         <v>0.1</v>
@@ -3330,35 +3326,35 @@
         <v>40</v>
       </c>
       <c r="O37" s="1">
-        <f>ROUNDUP(C37,0)</f>
-        <v>120</v>
+        <f t="shared" si="9"/>
+        <v>226</v>
       </c>
       <c r="P37" s="1">
-        <f>ROUNDUP(D37,0)</f>
+        <f t="shared" si="10"/>
         <v>18</v>
       </c>
       <c r="Q37" s="1">
-        <f>ROUNDUP(E37,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R37" s="1">
-        <f>ROUNDUP(F37,0)</f>
-        <v>1</v>
+        <f t="shared" si="12"/>
+        <v>2</v>
       </c>
       <c r="S37" s="1">
-        <f>ROUNDUP(G37,0)</f>
-        <v>4</v>
+        <f t="shared" si="13"/>
+        <v>2</v>
       </c>
       <c r="T37" s="1">
-        <f>ROUNDUP(H37,0)</f>
+        <f t="shared" si="14"/>
         <v>1</v>
       </c>
       <c r="U37" s="1">
-        <f>ROUNDUP(I37,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V37" s="1">
-        <f>ROUNDUP(J37,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W37" s="1">
@@ -3371,11 +3367,11 @@
         <v>0</v>
       </c>
       <c r="Z37" s="1">
-        <f>ROUNDUP(L37,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>18</v>
       </c>
@@ -3395,7 +3391,7 @@
         <v>0.25</v>
       </c>
       <c r="G38" s="1">
-        <v>0</v>
+        <v>0.37931034482758619</v>
       </c>
       <c r="H38" s="1">
         <v>5.2</v>
@@ -3416,35 +3412,35 @@
         <v>39</v>
       </c>
       <c r="O38" s="1">
-        <f>ROUNDUP(C38,0)</f>
+        <f t="shared" si="9"/>
         <v>27</v>
       </c>
       <c r="P38" s="1">
-        <f>ROUNDUP(D38,0)</f>
+        <f t="shared" si="10"/>
         <v>6</v>
       </c>
       <c r="Q38" s="1">
-        <f>ROUNDUP(E38,0)</f>
+        <f t="shared" si="11"/>
         <v>1</v>
       </c>
       <c r="R38" s="1">
-        <f>ROUNDUP(F38,0)</f>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="S38" s="1">
-        <f>ROUNDUP(G38,0)</f>
-        <v>0</v>
+        <f t="shared" si="13"/>
+        <v>1</v>
       </c>
       <c r="T38" s="1">
-        <f>ROUNDUP(H38,0)</f>
+        <f t="shared" si="14"/>
         <v>6</v>
       </c>
       <c r="U38" s="1">
-        <f>ROUNDUP(I38,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V38" s="1">
-        <f>ROUNDUP(J38,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W38" s="1">
@@ -3457,11 +3453,11 @@
         <v>0</v>
       </c>
       <c r="Z38" s="1">
-        <f>ROUNDUP(L38,0)</f>
+        <f t="shared" si="17"/>
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>38</v>
       </c>
@@ -3502,35 +3498,35 @@
         <v>37</v>
       </c>
       <c r="O39" s="1">
-        <f>ROUNDUP(C39,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P39" s="1">
-        <f>ROUNDUP(D39,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q39" s="1">
-        <f>ROUNDUP(E39,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R39" s="1">
-        <f>ROUNDUP(F39,0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S39" s="1">
-        <f>ROUNDUP(G39,0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T39" s="1">
-        <f>ROUNDUP(H39,0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U39" s="1">
-        <f>ROUNDUP(I39,0)</f>
+        <f t="shared" si="15"/>
         <v>0</v>
       </c>
       <c r="V39" s="1">
-        <f>ROUNDUP(J39,0)</f>
+        <f t="shared" si="16"/>
         <v>1</v>
       </c>
       <c r="W39" s="1">
@@ -3543,11 +3539,11 @@
         <v>0</v>
       </c>
       <c r="Z39" s="1">
-        <f>ROUNDUP(L39,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>36</v>
       </c>
@@ -3588,35 +3584,35 @@
         <v>35</v>
       </c>
       <c r="O40" s="1">
-        <f>ROUNDUP(C40,0)</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="P40" s="1">
-        <f>ROUNDUP(D40,0)</f>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="Q40" s="1">
-        <f>ROUNDUP(E40,0)</f>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="R40" s="1">
-        <f>ROUNDUP(F40,0)</f>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="S40" s="1">
-        <f>ROUNDUP(G40,0)</f>
+        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="T40" s="1">
-        <f>ROUNDUP(H40,0)</f>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="U40" s="1">
-        <f>ROUNDUP(I40,0)</f>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="V40" s="1">
-        <f>ROUNDUP(J40,0)</f>
+        <f t="shared" si="16"/>
         <v>0</v>
       </c>
       <c r="W40" s="1">
@@ -3629,21 +3625,21 @@
         <v>0</v>
       </c>
       <c r="Z40" s="1">
-        <f>ROUNDUP(L40,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="1:26" s="10" customFormat="1" ht="18" x14ac:dyDescent="0.35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" s="10" customFormat="1" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A42" s="11" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:26" x14ac:dyDescent="0.35">
       <c r="N44" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>33</v>
       </c>
@@ -3678,7 +3674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C46" s="1" t="s">
         <v>32</v>
       </c>
@@ -3746,7 +3742,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>28</v>
       </c>
@@ -3754,16 +3750,16 @@
         <v>27</v>
       </c>
       <c r="C47" s="1">
-        <v>297.69230800000003</v>
+        <v>297.69230769230768</v>
       </c>
       <c r="D47" s="1">
         <v>22.5</v>
       </c>
       <c r="E47" s="1">
-        <v>2.1758000000000002</v>
+        <v>2.1758241758241756</v>
       </c>
       <c r="F47" s="1">
-        <v>3.5769000000000002</v>
+        <v>3.5769230769230771</v>
       </c>
       <c r="G47" s="1">
         <v>0</v>
@@ -3787,35 +3783,35 @@
         <v>27</v>
       </c>
       <c r="O47" s="1">
-        <f>ROUNDUP(C47,0)</f>
+        <f t="shared" ref="O47:O57" si="18">ROUNDUP(C47,0)</f>
         <v>298</v>
       </c>
       <c r="P47" s="1">
-        <f>ROUNDUP(D47,0)</f>
+        <f t="shared" ref="P47:P57" si="19">ROUNDUP(D47,0)</f>
         <v>23</v>
       </c>
       <c r="Q47" s="1">
-        <f>ROUNDUP(E47,0)</f>
+        <f t="shared" ref="Q47:Q57" si="20">ROUNDUP(E47,0)</f>
         <v>3</v>
       </c>
       <c r="R47" s="1">
-        <f>ROUNDUP(F47,0)</f>
+        <f t="shared" ref="R47:R57" si="21">ROUNDUP(F47,0)</f>
         <v>4</v>
       </c>
       <c r="S47" s="1">
-        <f>ROUNDUP(G47,0)</f>
+        <f t="shared" ref="S47:S57" si="22">ROUNDUP(G47,0)</f>
         <v>0</v>
       </c>
       <c r="T47" s="1">
-        <f>ROUNDUP(H47,0)</f>
+        <f t="shared" ref="T47:T57" si="23">ROUNDUP(H47,0)</f>
         <v>0</v>
       </c>
       <c r="U47" s="1">
-        <f>ROUNDUP(I47,0)</f>
+        <f t="shared" ref="U47:U57" si="24">ROUNDUP(I47,0)</f>
         <v>0</v>
       </c>
       <c r="V47" s="1">
-        <f>ROUNDUP(J47,0)</f>
+        <f t="shared" ref="V47:V57" si="25">ROUNDUP(J47,0)</f>
         <v>0</v>
       </c>
       <c r="W47" s="1">
@@ -3828,11 +3824,11 @@
         <v>0</v>
       </c>
       <c r="Z47" s="1">
-        <f>ROUNDUP(L47,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Z47:Z57" si="26">ROUNDUP(L47,0)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>4</v>
       </c>
@@ -3840,16 +3836,16 @@
         <v>26</v>
       </c>
       <c r="C48" s="1">
-        <v>519.79894200000001</v>
+        <v>519.79894179894177</v>
       </c>
       <c r="D48" s="1">
-        <v>142.94999999999999</v>
+        <v>142.95238095238096</v>
       </c>
       <c r="E48" s="1">
-        <v>3.6190000000000002</v>
+        <v>3.6190476190476191</v>
       </c>
       <c r="F48" s="1">
-        <v>0.75929999999999997</v>
+        <v>0.7592592592592593</v>
       </c>
       <c r="G48" s="1">
         <v>0</v>
@@ -3873,35 +3869,35 @@
         <v>26</v>
       </c>
       <c r="O48" s="1">
-        <f>ROUNDUP(C48,0)</f>
+        <f t="shared" si="18"/>
         <v>520</v>
       </c>
       <c r="P48" s="1">
-        <f>ROUNDUP(D48,0)</f>
+        <f t="shared" si="19"/>
         <v>143</v>
       </c>
       <c r="Q48" s="1">
-        <f>ROUNDUP(E48,0)</f>
+        <f t="shared" si="20"/>
         <v>4</v>
       </c>
       <c r="R48" s="1">
-        <f>ROUNDUP(F48,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S48" s="1">
-        <f>ROUNDUP(G48,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T48" s="1">
-        <f>ROUNDUP(H48,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U48" s="1">
-        <f>ROUNDUP(I48,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V48" s="1">
-        <f>ROUNDUP(J48,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W48" s="1">
@@ -3914,11 +3910,11 @@
         <v>0</v>
       </c>
       <c r="Z48" s="1">
-        <f>ROUNDUP(L48,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>21</v>
       </c>
@@ -3926,16 +3922,16 @@
         <v>25</v>
       </c>
       <c r="C49" s="1">
-        <v>155.71590900000001</v>
+        <v>155.71590909090907</v>
       </c>
       <c r="D49" s="1">
-        <v>29.515000000000001</v>
+        <v>29.515151515151516</v>
       </c>
       <c r="E49" s="1">
-        <v>2.1212</v>
+        <v>2.1212121212121211</v>
       </c>
       <c r="F49" s="1">
-        <v>0.3977</v>
+        <v>0.39772727272727271</v>
       </c>
       <c r="G49" s="1">
         <v>0</v>
@@ -3959,35 +3955,35 @@
         <v>25</v>
       </c>
       <c r="O49" s="1">
-        <f>ROUNDUP(C49,0)</f>
+        <f t="shared" si="18"/>
         <v>156</v>
       </c>
       <c r="P49" s="1">
-        <f>ROUNDUP(D49,0)</f>
+        <f t="shared" si="19"/>
         <v>30</v>
       </c>
       <c r="Q49" s="1">
-        <f>ROUNDUP(E49,0)</f>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="R49" s="1">
-        <f>ROUNDUP(F49,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S49" s="1">
-        <f>ROUNDUP(G49,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T49" s="1">
-        <f>ROUNDUP(H49,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U49" s="1">
-        <f>ROUNDUP(I49,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V49" s="1">
-        <f>ROUNDUP(J49,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W49" s="1">
@@ -4000,11 +3996,11 @@
         <v>0</v>
       </c>
       <c r="Z49" s="1">
-        <f>ROUNDUP(L49,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>3</v>
       </c>
@@ -4012,16 +4008,16 @@
         <v>24</v>
       </c>
       <c r="C50" s="1">
-        <v>138.10638299999999</v>
+        <v>138.10638297872339</v>
       </c>
       <c r="D50" s="1">
         <v>28</v>
       </c>
       <c r="E50" s="1">
-        <v>2.5956999999999999</v>
+        <v>2.5957446808510638</v>
       </c>
       <c r="F50" s="1">
-        <v>0.38300000000000001</v>
+        <v>0.38297872340425532</v>
       </c>
       <c r="G50" s="1">
         <v>0</v>
@@ -4045,35 +4041,35 @@
         <v>24</v>
       </c>
       <c r="O50" s="1">
-        <f>ROUNDUP(C50,0)</f>
+        <f t="shared" si="18"/>
         <v>139</v>
       </c>
       <c r="P50" s="1">
-        <f>ROUNDUP(D50,0)</f>
+        <f t="shared" si="19"/>
         <v>28</v>
       </c>
       <c r="Q50" s="1">
-        <f>ROUNDUP(E50,0)</f>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="R50" s="1">
-        <f>ROUNDUP(F50,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S50" s="1">
-        <f>ROUNDUP(G50,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T50" s="1">
-        <f>ROUNDUP(H50,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U50" s="1">
-        <f>ROUNDUP(I50,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V50" s="1">
-        <f>ROUNDUP(J50,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W50" s="1">
@@ -4086,11 +4082,11 @@
         <v>0</v>
       </c>
       <c r="Z50" s="1">
-        <f>ROUNDUP(L50,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>20</v>
       </c>
@@ -4098,10 +4094,10 @@
         <v>23</v>
       </c>
       <c r="C51" s="1">
-        <v>82.666666699999993</v>
+        <v>82.666666666666671</v>
       </c>
       <c r="D51" s="1">
-        <v>18.082999999999998</v>
+        <v>18.083333333333332</v>
       </c>
       <c r="E51" s="1">
         <v>2</v>
@@ -4131,35 +4127,35 @@
         <v>23</v>
       </c>
       <c r="O51" s="1">
-        <f>ROUNDUP(C51,0)</f>
+        <f t="shared" si="18"/>
         <v>83</v>
       </c>
       <c r="P51" s="1">
-        <f>ROUNDUP(D51,0)</f>
+        <f t="shared" si="19"/>
         <v>19</v>
       </c>
       <c r="Q51" s="1">
-        <f>ROUNDUP(E51,0)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="R51" s="1">
-        <f>ROUNDUP(F51,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S51" s="1">
-        <f>ROUNDUP(G51,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T51" s="1">
-        <f>ROUNDUP(H51,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U51" s="1">
-        <f>ROUNDUP(I51,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V51" s="1">
-        <f>ROUNDUP(J51,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W51" s="1">
@@ -4172,11 +4168,11 @@
         <v>0</v>
       </c>
       <c r="Z51" s="1">
-        <f>ROUNDUP(L51,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>45</v>
       </c>
@@ -4184,19 +4180,19 @@
         <v>44</v>
       </c>
       <c r="C52" s="1">
-        <v>75.416666699999993</v>
+        <v>75.416666666666671</v>
       </c>
       <c r="D52" s="1">
-        <v>14.917</v>
+        <v>14.916666666666666</v>
       </c>
       <c r="E52" s="1">
         <v>2.25</v>
       </c>
       <c r="F52" s="1">
-        <v>8.3299999999999999E-2</v>
+        <v>8.3333333333333329E-2</v>
       </c>
       <c r="G52" s="1">
-        <v>4.1700000000000001E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="H52" s="1">
         <v>1</v>
@@ -4217,35 +4213,35 @@
         <v>44</v>
       </c>
       <c r="O52" s="1">
-        <f>ROUNDUP(C52,0)</f>
+        <f t="shared" si="18"/>
         <v>76</v>
       </c>
       <c r="P52" s="1">
-        <f>ROUNDUP(D52,0)</f>
+        <f t="shared" si="19"/>
         <v>15</v>
       </c>
       <c r="Q52" s="1">
-        <f>ROUNDUP(E52,0)</f>
+        <f t="shared" si="20"/>
         <v>3</v>
       </c>
       <c r="R52" s="1">
-        <f>ROUNDUP(F52,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S52" s="1">
-        <f>ROUNDUP(G52,0)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="T52" s="1">
-        <f>ROUNDUP(H52,0)</f>
+        <f t="shared" si="23"/>
         <v>1</v>
       </c>
       <c r="U52" s="1">
-        <f>ROUNDUP(I52,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V52" s="1">
-        <f>ROUNDUP(J52,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W52" s="1">
@@ -4258,11 +4254,11 @@
         <v>0</v>
       </c>
       <c r="Z52" s="1">
-        <f>ROUNDUP(L52,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>43</v>
       </c>
@@ -4303,35 +4299,35 @@
         <v>42</v>
       </c>
       <c r="O53" s="1">
-        <f>ROUNDUP(C53,0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P53" s="1">
-        <f>ROUNDUP(D53,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q53" s="1">
-        <f>ROUNDUP(E53,0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R53" s="1">
-        <f>ROUNDUP(F53,0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S53" s="1">
-        <f>ROUNDUP(G53,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T53" s="1">
-        <f>ROUNDUP(H53,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U53" s="1">
-        <f>ROUNDUP(I53,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V53" s="1">
-        <f>ROUNDUP(J53,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W53" s="1">
@@ -4344,11 +4340,11 @@
         <v>0</v>
       </c>
       <c r="Z53" s="1">
-        <f>ROUNDUP(L53,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>41</v>
       </c>
@@ -4356,16 +4352,16 @@
         <v>40</v>
       </c>
       <c r="C54" s="1">
-        <v>116.333333</v>
+        <v>116.33333333333333</v>
       </c>
       <c r="D54" s="1">
         <v>23</v>
       </c>
       <c r="E54" s="1">
-        <v>1.8332999999999999</v>
+        <v>1.8333333333333333</v>
       </c>
       <c r="F54" s="1">
-        <v>0.16669999999999999</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="G54" s="1">
         <v>1</v>
@@ -4389,35 +4385,35 @@
         <v>40</v>
       </c>
       <c r="O54" s="1">
-        <f>ROUNDUP(C54,0)</f>
+        <f t="shared" si="18"/>
         <v>117</v>
       </c>
       <c r="P54" s="1">
-        <f>ROUNDUP(D54,0)</f>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
       <c r="Q54" s="1">
-        <f>ROUNDUP(E54,0)</f>
+        <f t="shared" si="20"/>
         <v>2</v>
       </c>
       <c r="R54" s="1">
-        <f>ROUNDUP(F54,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S54" s="1">
-        <f>ROUNDUP(G54,0)</f>
+        <f t="shared" si="22"/>
         <v>1</v>
       </c>
       <c r="T54" s="1">
-        <f>ROUNDUP(H54,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U54" s="1">
-        <f>ROUNDUP(I54,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V54" s="1">
-        <f>ROUNDUP(J54,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W54" s="1">
@@ -4430,11 +4426,11 @@
         <v>0</v>
       </c>
       <c r="Z54" s="1">
-        <f>ROUNDUP(L54,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>18</v>
       </c>
@@ -4475,35 +4471,35 @@
         <v>39</v>
       </c>
       <c r="O55" s="1">
-        <f>ROUNDUP(C55,0)</f>
+        <f t="shared" si="18"/>
         <v>115</v>
       </c>
       <c r="P55" s="1">
-        <f>ROUNDUP(D55,0)</f>
+        <f t="shared" si="19"/>
         <v>23</v>
       </c>
       <c r="Q55" s="1">
-        <f>ROUNDUP(E55,0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R55" s="1">
-        <f>ROUNDUP(F55,0)</f>
+        <f t="shared" si="21"/>
         <v>1</v>
       </c>
       <c r="S55" s="1">
-        <f>ROUNDUP(G55,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T55" s="1">
-        <f>ROUNDUP(H55,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U55" s="1">
-        <f>ROUNDUP(I55,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V55" s="1">
-        <f>ROUNDUP(J55,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W55" s="1">
@@ -4516,11 +4512,11 @@
         <v>0</v>
       </c>
       <c r="Z55" s="1">
-        <f>ROUNDUP(L55,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>38</v>
       </c>
@@ -4561,35 +4557,35 @@
         <v>37</v>
       </c>
       <c r="O56" s="1">
-        <f>ROUNDUP(C56,0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P56" s="1">
-        <f>ROUNDUP(D56,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q56" s="1">
-        <f>ROUNDUP(E56,0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R56" s="1">
-        <f>ROUNDUP(F56,0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S56" s="1">
-        <f>ROUNDUP(G56,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T56" s="1">
-        <f>ROUNDUP(H56,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U56" s="1">
-        <f>ROUNDUP(I56,0)</f>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="V56" s="1">
-        <f>ROUNDUP(J56,0)</f>
+        <f t="shared" si="25"/>
         <v>1</v>
       </c>
       <c r="W56" s="1">
@@ -4602,11 +4598,11 @@
         <v>0</v>
       </c>
       <c r="Z56" s="1">
-        <f>ROUNDUP(L56,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>36</v>
       </c>
@@ -4647,35 +4643,35 @@
         <v>35</v>
       </c>
       <c r="O57" s="1">
-        <f>ROUNDUP(C57,0)</f>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="P57" s="1">
-        <f>ROUNDUP(D57,0)</f>
+        <f t="shared" si="19"/>
         <v>0</v>
       </c>
       <c r="Q57" s="1">
-        <f>ROUNDUP(E57,0)</f>
+        <f t="shared" si="20"/>
         <v>0</v>
       </c>
       <c r="R57" s="1">
-        <f>ROUNDUP(F57,0)</f>
+        <f t="shared" si="21"/>
         <v>0</v>
       </c>
       <c r="S57" s="1">
-        <f>ROUNDUP(G57,0)</f>
+        <f t="shared" si="22"/>
         <v>0</v>
       </c>
       <c r="T57" s="1">
-        <f>ROUNDUP(H57,0)</f>
+        <f t="shared" si="23"/>
         <v>0</v>
       </c>
       <c r="U57" s="1">
-        <f>ROUNDUP(I57,0)</f>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="V57" s="1">
-        <f>ROUNDUP(J57,0)</f>
+        <f t="shared" si="25"/>
         <v>0</v>
       </c>
       <c r="W57" s="1">
@@ -4688,11 +4684,11 @@
         <v>0</v>
       </c>
       <c r="Z57" s="1">
-        <f>ROUNDUP(L57,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="26"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>29</v>
       </c>
@@ -4757,7 +4753,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:26" x14ac:dyDescent="0.35">
       <c r="C63" s="1" t="s">
         <v>32</v>
       </c>
@@ -4825,7 +4821,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>28</v>
       </c>
@@ -4833,19 +4829,19 @@
         <v>27</v>
       </c>
       <c r="C64" s="1">
-        <v>297.69230800000003</v>
+        <v>297.69230769230768</v>
       </c>
       <c r="D64" s="1">
-        <v>26.213999999999999</v>
+        <v>22.5</v>
       </c>
       <c r="E64" s="1">
-        <v>4.0713999999999997</v>
+        <v>2.2409638554216866</v>
       </c>
       <c r="F64" s="1">
-        <v>3.5769000000000002</v>
+        <v>3.5769230769230771</v>
       </c>
       <c r="G64" s="1">
-        <v>0</v>
+        <v>1.2048192771084338E-2</v>
       </c>
       <c r="H64" s="1">
         <v>0.39</v>
@@ -4866,35 +4862,35 @@
         <v>27</v>
       </c>
       <c r="O64" s="1">
-        <f>ROUNDUP(C64,0)</f>
+        <f t="shared" ref="O64:O74" si="27">ROUNDUP(C64,0)</f>
         <v>298</v>
       </c>
       <c r="P64" s="1">
-        <f>ROUNDUP(D64,0)</f>
-        <v>27</v>
+        <f t="shared" ref="P64:P74" si="28">ROUNDUP(D64,0)</f>
+        <v>23</v>
       </c>
       <c r="Q64" s="1">
-        <f>ROUNDUP(E64,0)</f>
-        <v>5</v>
+        <f t="shared" ref="Q64:Q74" si="29">ROUNDUP(E64,0)</f>
+        <v>3</v>
       </c>
       <c r="R64" s="1">
-        <f>ROUNDUP(F64,0)</f>
+        <f t="shared" ref="R64:R74" si="30">ROUNDUP(F64,0)</f>
         <v>4</v>
       </c>
       <c r="S64" s="1">
-        <f>ROUNDUP(G64,0)</f>
-        <v>0</v>
+        <f t="shared" ref="S64:S74" si="31">ROUNDUP(G64,0)</f>
+        <v>1</v>
       </c>
       <c r="T64" s="1">
-        <f>ROUNDUP(H64,0)</f>
+        <f t="shared" ref="T64:T74" si="32">ROUNDUP(H64,0)</f>
         <v>1</v>
       </c>
       <c r="U64" s="1">
-        <f>ROUNDUP(I64,0)</f>
+        <f t="shared" ref="U64:U74" si="33">ROUNDUP(I64,0)</f>
         <v>0</v>
       </c>
       <c r="V64" s="1">
-        <f>ROUNDUP(J64,0)</f>
+        <f t="shared" ref="V64:V74" si="34">ROUNDUP(J64,0)</f>
         <v>0</v>
       </c>
       <c r="W64" s="1">
@@ -4907,11 +4903,11 @@
         <v>0</v>
       </c>
       <c r="Z64" s="1">
-        <f>ROUNDUP(L64,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" ref="Z64:Z74" si="35">ROUNDUP(L64,0)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>4</v>
       </c>
@@ -4919,16 +4915,16 @@
         <v>26</v>
       </c>
       <c r="C65" s="1">
-        <v>117.22037</v>
+        <v>121.44179894179894</v>
       </c>
       <c r="D65" s="1">
         <v>28.67</v>
       </c>
       <c r="E65" s="1">
-        <v>2.76</v>
+        <v>4.0714285714285712</v>
       </c>
       <c r="F65" s="1">
-        <v>0.94</v>
+        <v>0.7592592592592593</v>
       </c>
       <c r="G65" s="1">
         <v>0</v>
@@ -4952,35 +4948,35 @@
         <v>26</v>
       </c>
       <c r="O65" s="1">
-        <f>ROUNDUP(C65,0)</f>
-        <v>118</v>
+        <f t="shared" si="27"/>
+        <v>122</v>
       </c>
       <c r="P65" s="1">
-        <f>ROUNDUP(D65,0)</f>
+        <f t="shared" si="28"/>
         <v>29</v>
       </c>
       <c r="Q65" s="1">
-        <f>ROUNDUP(E65,0)</f>
-        <v>3</v>
+        <f t="shared" si="29"/>
+        <v>5</v>
       </c>
       <c r="R65" s="1">
-        <f>ROUNDUP(F65,0)</f>
+        <f t="shared" si="30"/>
         <v>1</v>
       </c>
       <c r="S65" s="1">
-        <f>ROUNDUP(G65,0)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="T65" s="1">
-        <f>ROUNDUP(H65,0)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="U65" s="1">
-        <f>ROUNDUP(I65,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V65" s="1">
-        <f>ROUNDUP(J65,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W65" s="1">
@@ -4993,11 +4989,11 @@
         <v>0</v>
       </c>
       <c r="Z65" s="1">
-        <f>ROUNDUP(L65,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>21</v>
       </c>
@@ -5005,19 +5001,19 @@
         <v>25</v>
       </c>
       <c r="C66" s="1">
-        <v>176.37805299999999</v>
+        <v>116.73954545454545</v>
       </c>
       <c r="D66" s="1">
-        <v>28.552</v>
+        <v>18.65909090909091</v>
       </c>
       <c r="E66" s="1">
-        <v>4.9402999999999997</v>
+        <v>2.76</v>
       </c>
       <c r="F66" s="1">
-        <v>1.9402999999999999</v>
+        <v>0.94</v>
       </c>
       <c r="G66" s="1">
-        <v>0.1343</v>
+        <v>0</v>
       </c>
       <c r="H66" s="1">
         <v>3.73</v>
@@ -5038,35 +5034,35 @@
         <v>25</v>
       </c>
       <c r="O66" s="1">
-        <f>ROUNDUP(C66,0)</f>
-        <v>177</v>
+        <f t="shared" si="27"/>
+        <v>117</v>
       </c>
       <c r="P66" s="1">
-        <f>ROUNDUP(D66,0)</f>
-        <v>29</v>
+        <f t="shared" si="28"/>
+        <v>19</v>
       </c>
       <c r="Q66" s="1">
-        <f>ROUNDUP(E66,0)</f>
-        <v>5</v>
+        <f t="shared" si="29"/>
+        <v>3</v>
       </c>
       <c r="R66" s="1">
-        <f>ROUNDUP(F66,0)</f>
-        <v>2</v>
+        <f t="shared" si="30"/>
+        <v>1</v>
       </c>
       <c r="S66" s="1">
-        <f>ROUNDUP(G66,0)</f>
-        <v>1</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="T66" s="1">
-        <f>ROUNDUP(H66,0)</f>
+        <f t="shared" si="32"/>
         <v>4</v>
       </c>
       <c r="U66" s="1">
-        <f>ROUNDUP(I66,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V66" s="1">
-        <f>ROUNDUP(J66,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W66" s="1">
@@ -5079,11 +5075,11 @@
         <v>0</v>
       </c>
       <c r="Z66" s="1">
-        <f>ROUNDUP(L66,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>3</v>
       </c>
@@ -5091,19 +5087,19 @@
         <v>24</v>
       </c>
       <c r="C67" s="1">
-        <v>124.93</v>
+        <v>179.29850746268656</v>
       </c>
       <c r="D67" s="1">
-        <v>28</v>
+        <v>28.552238805970148</v>
       </c>
       <c r="E67" s="1">
-        <v>0.75</v>
+        <v>4.9402985074626864</v>
       </c>
       <c r="F67" s="1">
-        <v>1.6</v>
+        <v>1.9402985074626866</v>
       </c>
       <c r="G67" s="1">
-        <v>0</v>
+        <v>0.13432835820895522</v>
       </c>
       <c r="H67" s="1">
         <v>2.39</v>
@@ -5124,35 +5120,35 @@
         <v>24</v>
       </c>
       <c r="O67" s="1">
-        <f>ROUNDUP(C67,0)</f>
-        <v>125</v>
+        <f t="shared" si="27"/>
+        <v>180</v>
       </c>
       <c r="P67" s="1">
-        <f>ROUNDUP(D67,0)</f>
-        <v>28</v>
+        <f t="shared" si="28"/>
+        <v>29</v>
       </c>
       <c r="Q67" s="1">
-        <f>ROUNDUP(E67,0)</f>
-        <v>1</v>
+        <f t="shared" si="29"/>
+        <v>5</v>
       </c>
       <c r="R67" s="1">
-        <f>ROUNDUP(F67,0)</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="S67" s="1">
-        <f>ROUNDUP(G67,0)</f>
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>1</v>
       </c>
       <c r="T67" s="1">
-        <f>ROUNDUP(H67,0)</f>
+        <f t="shared" si="32"/>
         <v>3</v>
       </c>
       <c r="U67" s="1">
-        <f>ROUNDUP(I67,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V67" s="1">
-        <f>ROUNDUP(J67,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W67" s="1">
@@ -5165,11 +5161,11 @@
         <v>0</v>
       </c>
       <c r="Z67" s="1">
-        <f>ROUNDUP(L67,0)</f>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
     </row>
-    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>20</v>
       </c>
@@ -5186,7 +5182,7 @@
         <v>2</v>
       </c>
       <c r="F68" s="1">
-        <v>1.07</v>
+        <v>1.5</v>
       </c>
       <c r="G68" s="1">
         <v>0</v>
@@ -5210,35 +5206,35 @@
         <v>23</v>
       </c>
       <c r="O68" s="1">
-        <f>ROUNDUP(C68,0)</f>
+        <f t="shared" si="27"/>
         <v>100</v>
       </c>
       <c r="P68" s="1">
-        <f>ROUNDUP(D68,0)</f>
+        <f t="shared" si="28"/>
         <v>19</v>
       </c>
       <c r="Q68" s="1">
-        <f>ROUNDUP(E68,0)</f>
+        <f t="shared" si="29"/>
         <v>2</v>
       </c>
       <c r="R68" s="1">
-        <f>ROUNDUP(F68,0)</f>
+        <f t="shared" si="30"/>
         <v>2</v>
       </c>
       <c r="S68" s="1">
-        <f>ROUNDUP(G68,0)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="T68" s="1">
-        <f>ROUNDUP(H68,0)</f>
+        <f t="shared" si="32"/>
         <v>2</v>
       </c>
       <c r="U68" s="1">
-        <f>ROUNDUP(I68,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V68" s="1">
-        <f>ROUNDUP(J68,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W68" s="1">
@@ -5251,11 +5247,11 @@
         <v>0</v>
       </c>
       <c r="Z68" s="1">
-        <f>ROUNDUP(L68,0)</f>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
     </row>
-    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>45</v>
       </c>
@@ -5263,19 +5259,19 @@
         <v>44</v>
       </c>
       <c r="C69" s="1">
-        <v>178.25</v>
+        <v>53.171428571428571</v>
       </c>
       <c r="D69" s="1">
-        <v>30.25</v>
+        <v>6.9428571428571431</v>
       </c>
       <c r="E69" s="1">
-        <v>8.75</v>
+        <v>1.6285714285714286</v>
       </c>
       <c r="F69" s="1">
-        <v>13.5</v>
+        <v>0.23</v>
       </c>
       <c r="G69" s="1">
-        <v>1.25</v>
+        <v>0</v>
       </c>
       <c r="H69" s="1">
         <v>0.23</v>
@@ -5296,35 +5292,35 @@
         <v>44</v>
       </c>
       <c r="O69" s="1">
-        <f>ROUNDUP(C69,0)</f>
-        <v>179</v>
+        <f t="shared" si="27"/>
+        <v>54</v>
       </c>
       <c r="P69" s="1">
-        <f>ROUNDUP(D69,0)</f>
-        <v>31</v>
+        <f t="shared" si="28"/>
+        <v>7</v>
       </c>
       <c r="Q69" s="1">
-        <f>ROUNDUP(E69,0)</f>
-        <v>9</v>
+        <f t="shared" si="29"/>
+        <v>2</v>
       </c>
       <c r="R69" s="1">
-        <f>ROUNDUP(F69,0)</f>
-        <v>14</v>
+        <f t="shared" si="30"/>
+        <v>1</v>
       </c>
       <c r="S69" s="1">
-        <f>ROUNDUP(G69,0)</f>
-        <v>2</v>
+        <f t="shared" si="31"/>
+        <v>0</v>
       </c>
       <c r="T69" s="1">
-        <f>ROUNDUP(H69,0)</f>
+        <f t="shared" si="32"/>
         <v>1</v>
       </c>
       <c r="U69" s="1">
-        <f>ROUNDUP(I69,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V69" s="1">
-        <f>ROUNDUP(J69,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W69" s="1">
@@ -5337,11 +5333,11 @@
         <v>0</v>
       </c>
       <c r="Z69" s="1">
-        <f>ROUNDUP(L69,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>43</v>
       </c>
@@ -5382,35 +5378,35 @@
         <v>42</v>
       </c>
       <c r="O70" s="1">
-        <f>ROUNDUP(C70,0)</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P70" s="1">
-        <f>ROUNDUP(D70,0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q70" s="1">
-        <f>ROUNDUP(E70,0)</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R70" s="1">
-        <f>ROUNDUP(F70,0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="S70" s="1">
-        <f>ROUNDUP(G70,0)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="T70" s="1">
-        <f>ROUNDUP(H70,0)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U70" s="1">
-        <f>ROUNDUP(I70,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V70" s="1">
-        <f>ROUNDUP(J70,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W70" s="1">
@@ -5423,11 +5419,11 @@
         <v>0</v>
       </c>
       <c r="Z70" s="1">
-        <f>ROUNDUP(L70,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>41</v>
       </c>
@@ -5441,7 +5437,7 @@
         <v>34.450000000000003</v>
       </c>
       <c r="E71" s="1">
-        <v>4</v>
+        <v>4.833333333333333</v>
       </c>
       <c r="F71" s="1">
         <v>3.51</v>
@@ -5468,35 +5464,35 @@
         <v>40</v>
       </c>
       <c r="O71" s="1">
-        <f>ROUNDUP(C71,0)</f>
+        <f t="shared" si="27"/>
         <v>586</v>
       </c>
       <c r="P71" s="1">
-        <f>ROUNDUP(D71,0)</f>
+        <f t="shared" si="28"/>
         <v>35</v>
       </c>
       <c r="Q71" s="1">
-        <f>ROUNDUP(E71,0)</f>
+        <f t="shared" si="29"/>
+        <v>5</v>
+      </c>
+      <c r="R71" s="1">
+        <f t="shared" si="30"/>
         <v>4</v>
       </c>
-      <c r="R71" s="1">
-        <f>ROUNDUP(F71,0)</f>
+      <c r="S71" s="1">
+        <f t="shared" si="31"/>
         <v>4</v>
       </c>
-      <c r="S71" s="1">
-        <f>ROUNDUP(G71,0)</f>
-        <v>4</v>
-      </c>
       <c r="T71" s="1">
-        <f>ROUNDUP(H71,0)</f>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="U71" s="1">
-        <f>ROUNDUP(I71,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V71" s="1">
-        <f>ROUNDUP(J71,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W71" s="1">
@@ -5509,11 +5505,11 @@
         <v>0</v>
       </c>
       <c r="Z71" s="1">
-        <f>ROUNDUP(L71,0)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="35"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>18</v>
       </c>
@@ -5524,16 +5520,16 @@
         <v>217</v>
       </c>
       <c r="D72" s="1">
-        <v>28.84</v>
+        <v>28.931034482758619</v>
       </c>
       <c r="E72" s="1">
-        <v>0.4</v>
+        <v>4.3103448275862073</v>
       </c>
       <c r="F72" s="1">
-        <v>2.4900000000000002</v>
+        <v>2.5172413793103448</v>
       </c>
       <c r="G72" s="1">
-        <v>0</v>
+        <v>0.37931034482758619</v>
       </c>
       <c r="H72" s="1">
         <v>5.2</v>
@@ -5554,35 +5550,35 @@
         <v>39</v>
       </c>
       <c r="O72" s="1">
-        <f>ROUNDUP(C72,0)</f>
+        <f t="shared" si="27"/>
         <v>217</v>
       </c>
       <c r="P72" s="1">
-        <f>ROUNDUP(D72,0)</f>
+        <f t="shared" si="28"/>
         <v>29</v>
       </c>
       <c r="Q72" s="1">
-        <f>ROUNDUP(E72,0)</f>
-        <v>1</v>
+        <f t="shared" si="29"/>
+        <v>5</v>
       </c>
       <c r="R72" s="1">
-        <f>ROUNDUP(F72,0)</f>
+        <f t="shared" si="30"/>
         <v>3</v>
       </c>
       <c r="S72" s="1">
-        <f>ROUNDUP(G72,0)</f>
-        <v>0</v>
+        <f t="shared" si="31"/>
+        <v>1</v>
       </c>
       <c r="T72" s="1">
-        <f>ROUNDUP(H72,0)</f>
+        <f t="shared" si="32"/>
         <v>6</v>
       </c>
       <c r="U72" s="1">
-        <f>ROUNDUP(I72,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V72" s="1">
-        <f>ROUNDUP(J72,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W72" s="1">
@@ -5595,11 +5591,11 @@
         <v>0</v>
       </c>
       <c r="Z72" s="1">
-        <f>ROUNDUP(L72,0)</f>
+        <f t="shared" si="35"/>
         <v>2</v>
       </c>
     </row>
-    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>38</v>
       </c>
@@ -5640,35 +5636,35 @@
         <v>37</v>
       </c>
       <c r="O73" s="1">
-        <f>ROUNDUP(C73,0)</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P73" s="1">
-        <f>ROUNDUP(D73,0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q73" s="1">
-        <f>ROUNDUP(E73,0)</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R73" s="1">
-        <f>ROUNDUP(F73,0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="S73" s="1">
-        <f>ROUNDUP(G73,0)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="T73" s="1">
-        <f>ROUNDUP(H73,0)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U73" s="1">
-        <f>ROUNDUP(I73,0)</f>
+        <f t="shared" si="33"/>
         <v>0</v>
       </c>
       <c r="V73" s="1">
-        <f>ROUNDUP(J73,0)</f>
+        <f t="shared" si="34"/>
         <v>1</v>
       </c>
       <c r="W73" s="1">
@@ -5681,11 +5677,11 @@
         <v>0</v>
       </c>
       <c r="Z73" s="1">
-        <f>ROUNDUP(L73,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>36</v>
       </c>
@@ -5726,35 +5722,35 @@
         <v>35</v>
       </c>
       <c r="O74" s="1">
-        <f>ROUNDUP(C74,0)</f>
+        <f t="shared" si="27"/>
         <v>0</v>
       </c>
       <c r="P74" s="1">
-        <f>ROUNDUP(D74,0)</f>
+        <f t="shared" si="28"/>
         <v>0</v>
       </c>
       <c r="Q74" s="1">
-        <f>ROUNDUP(E74,0)</f>
+        <f t="shared" si="29"/>
         <v>0</v>
       </c>
       <c r="R74" s="1">
-        <f>ROUNDUP(F74,0)</f>
+        <f t="shared" si="30"/>
         <v>0</v>
       </c>
       <c r="S74" s="1">
-        <f>ROUNDUP(G74,0)</f>
+        <f t="shared" si="31"/>
         <v>0</v>
       </c>
       <c r="T74" s="1">
-        <f>ROUNDUP(H74,0)</f>
+        <f t="shared" si="32"/>
         <v>0</v>
       </c>
       <c r="U74" s="1">
-        <f>ROUNDUP(I74,0)</f>
+        <f t="shared" si="33"/>
         <v>1</v>
       </c>
       <c r="V74" s="1">
-        <f>ROUNDUP(J74,0)</f>
+        <f t="shared" si="34"/>
         <v>0</v>
       </c>
       <c r="W74" s="1">
@@ -5767,16 +5763,16 @@
         <v>0</v>
       </c>
       <c r="Z74" s="1">
-        <f>ROUNDUP(L74,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:26" ht="18" x14ac:dyDescent="0.35">
+        <f t="shared" si="35"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:26" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A76" s="9" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>33</v>
       </c>
@@ -5790,8 +5786,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="79" spans="1:26" ht="15.6" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" ht="15.65" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row r="80" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>28</v>
       </c>
@@ -5799,39 +5795,39 @@
         <v>27</v>
       </c>
       <c r="O80" s="1">
-        <f>CEILING(AVERAGE(O47,O13),1)</f>
+        <f t="shared" ref="O80:W80" si="36">CEILING(AVERAGE(O47,O13),1)</f>
         <v>180</v>
       </c>
       <c r="P80" s="1">
-        <f>CEILING(AVERAGE(P47,P13),1)</f>
+        <f t="shared" si="36"/>
         <v>15</v>
       </c>
       <c r="Q80" s="1">
-        <f>CEILING(AVERAGE(Q47,Q13),1)</f>
+        <f t="shared" si="36"/>
         <v>2</v>
       </c>
       <c r="R80" s="1">
-        <f>CEILING(AVERAGE(R47,R13),1)</f>
+        <f t="shared" si="36"/>
         <v>3</v>
       </c>
       <c r="S80" s="1">
-        <f>CEILING(AVERAGE(S47,S13),1)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="T80" s="1">
-        <f>CEILING(AVERAGE(T47,T13),1)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="U80" s="1">
-        <f>CEILING(AVERAGE(U47,U13),1)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="V80" s="1">
-        <f>CEILING(AVERAGE(V47,V13),1)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="W80" s="1">
-        <f>CEILING(AVERAGE(W47,W13),1)</f>
+        <f t="shared" si="36"/>
         <v>0</v>
       </c>
       <c r="Z80" s="1">
@@ -5839,7 +5835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>4</v>
       </c>
@@ -5847,39 +5843,39 @@
         <v>26</v>
       </c>
       <c r="O81" s="1">
-        <f>CEILING(AVERAGE(O48,O14),1)</f>
+        <f t="shared" ref="O81:W81" si="37">CEILING(AVERAGE(O48,O14),1)</f>
         <v>272</v>
       </c>
       <c r="P81" s="1">
-        <f>CEILING(AVERAGE(P48,P14),1)</f>
+        <f t="shared" si="37"/>
         <v>73</v>
       </c>
       <c r="Q81" s="1">
-        <f>CEILING(AVERAGE(Q48,Q14),1)</f>
+        <f t="shared" si="37"/>
         <v>3</v>
       </c>
       <c r="R81" s="1">
-        <f>CEILING(AVERAGE(R48,R14),1)</f>
+        <f t="shared" si="37"/>
         <v>1</v>
       </c>
       <c r="S81" s="1">
-        <f>CEILING(AVERAGE(S48,S14),1)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="T81" s="1">
-        <f>CEILING(AVERAGE(T48,T14),1)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="U81" s="1">
-        <f>CEILING(AVERAGE(U48,U14),1)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="V81" s="1">
-        <f>CEILING(AVERAGE(V48,V14),1)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="W81" s="1">
-        <f>CEILING(AVERAGE(W48,W14),1)</f>
+        <f t="shared" si="37"/>
         <v>0</v>
       </c>
       <c r="Z81" s="1">
@@ -5887,7 +5883,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>21</v>
       </c>
@@ -5895,39 +5891,39 @@
         <v>25</v>
       </c>
       <c r="O82" s="1">
-        <f>CEILING(AVERAGE(O49,O15),1)</f>
+        <f t="shared" ref="O82:W82" si="38">CEILING(AVERAGE(O49,O15),1)</f>
         <v>93</v>
       </c>
       <c r="P82" s="1">
-        <f>CEILING(AVERAGE(P49,P15),1)</f>
+        <f t="shared" si="38"/>
         <v>17</v>
       </c>
       <c r="Q82" s="1">
-        <f>CEILING(AVERAGE(Q49,Q15),1)</f>
+        <f t="shared" si="38"/>
         <v>2</v>
       </c>
       <c r="R82" s="1">
-        <f>CEILING(AVERAGE(R49,R15),1)</f>
+        <f t="shared" si="38"/>
         <v>1</v>
       </c>
       <c r="S82" s="1">
-        <f>CEILING(AVERAGE(S49,S15),1)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="T82" s="1">
-        <f>CEILING(AVERAGE(T49,T15),1)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="U82" s="1">
-        <f>CEILING(AVERAGE(U49,U15),1)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="V82" s="1">
-        <f>CEILING(AVERAGE(V49,V15),1)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="W82" s="1">
-        <f>CEILING(AVERAGE(W49,W15),1)</f>
+        <f t="shared" si="38"/>
         <v>0</v>
       </c>
       <c r="Z82" s="1">
@@ -5935,7 +5931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>3</v>
       </c>
@@ -5943,39 +5939,39 @@
         <v>24</v>
       </c>
       <c r="O83" s="1">
-        <f>CEILING(AVERAGE(O50,O16),1)</f>
+        <f t="shared" ref="O83:W83" si="39">CEILING(AVERAGE(O50,O16),1)</f>
         <v>101</v>
       </c>
       <c r="P83" s="1">
-        <f>CEILING(AVERAGE(P50,P16),1)</f>
+        <f t="shared" si="39"/>
         <v>20</v>
       </c>
       <c r="Q83" s="1">
-        <f>CEILING(AVERAGE(Q50,Q16),1)</f>
+        <f t="shared" si="39"/>
         <v>3</v>
       </c>
       <c r="R83" s="1">
-        <f>CEILING(AVERAGE(R50,R16),1)</f>
+        <f t="shared" si="39"/>
         <v>1</v>
       </c>
       <c r="S83" s="1">
-        <f>CEILING(AVERAGE(S50,S16),1)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="T83" s="1">
-        <f>CEILING(AVERAGE(T50,T16),1)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="U83" s="1">
-        <f>CEILING(AVERAGE(U50,U16),1)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="V83" s="1">
-        <f>CEILING(AVERAGE(V50,V16),1)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="W83" s="1">
-        <f>CEILING(AVERAGE(W50,W16),1)</f>
+        <f t="shared" si="39"/>
         <v>0</v>
       </c>
       <c r="Z83" s="1">
@@ -5983,7 +5979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>20</v>
       </c>
@@ -5991,39 +5987,39 @@
         <v>23</v>
       </c>
       <c r="O84" s="1">
-        <f>CEILING(AVERAGE(O51,O17),1)</f>
+        <f t="shared" ref="O84:W84" si="40">CEILING(AVERAGE(O51,O17),1)</f>
         <v>49</v>
       </c>
       <c r="P84" s="1">
-        <f>CEILING(AVERAGE(P51,P17),1)</f>
+        <f t="shared" si="40"/>
         <v>10</v>
       </c>
       <c r="Q84" s="1">
-        <f>CEILING(AVERAGE(Q51,Q17),1)</f>
+        <f t="shared" si="40"/>
         <v>2</v>
       </c>
       <c r="R84" s="1">
-        <f>CEILING(AVERAGE(R51,R17),1)</f>
+        <f t="shared" si="40"/>
         <v>1</v>
       </c>
       <c r="S84" s="1">
-        <f>CEILING(AVERAGE(S51,S17),1)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="T84" s="1">
-        <f>CEILING(AVERAGE(T51,T17),1)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="U84" s="1">
-        <f>CEILING(AVERAGE(U51,U17),1)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="V84" s="1">
-        <f>CEILING(AVERAGE(V51,V17),1)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="W84" s="1">
-        <f>CEILING(AVERAGE(W51,W17),1)</f>
+        <f t="shared" si="40"/>
         <v>0</v>
       </c>
       <c r="Z84" s="1">
@@ -6031,12 +6027,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>28</v>
       </c>
@@ -6044,39 +6040,39 @@
         <v>27</v>
       </c>
       <c r="O89" s="1">
-        <f>CEILING(AVERAGE(O64,O30),1)</f>
-        <v>186</v>
+        <f t="shared" ref="O89:W89" si="41">CEILING(AVERAGE(O64,O30),1)</f>
+        <v>184</v>
       </c>
       <c r="P89" s="1">
-        <f>CEILING(AVERAGE(P64,P30),1)</f>
-        <v>20</v>
+        <f t="shared" si="41"/>
+        <v>18</v>
       </c>
       <c r="Q89" s="1">
-        <f>CEILING(AVERAGE(Q64,Q30),1)</f>
+        <f t="shared" si="41"/>
+        <v>2</v>
+      </c>
+      <c r="R89" s="1">
+        <f t="shared" si="41"/>
         <v>3</v>
       </c>
-      <c r="R89" s="1">
-        <f>CEILING(AVERAGE(R64,R30),1)</f>
-        <v>3</v>
-      </c>
       <c r="S89" s="1">
-        <f>CEILING(AVERAGE(S64,S30),1)</f>
-        <v>0</v>
+        <f t="shared" si="41"/>
+        <v>1</v>
       </c>
       <c r="T89" s="1">
-        <f>CEILING(AVERAGE(T64,T30),1)</f>
+        <f t="shared" si="41"/>
         <v>1</v>
       </c>
       <c r="U89" s="1">
-        <f>CEILING(AVERAGE(U64,U30),1)</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="V89" s="1">
-        <f>CEILING(AVERAGE(V64,V30),1)</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="W89" s="1">
-        <f>CEILING(AVERAGE(W64,W30),1)</f>
+        <f t="shared" si="41"/>
         <v>0</v>
       </c>
       <c r="Z89" s="1">
@@ -6084,7 +6080,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>4</v>
       </c>
@@ -6092,39 +6088,39 @@
         <v>26</v>
       </c>
       <c r="O90" s="1">
-        <f>CEILING(AVERAGE(O65,O31),1)</f>
-        <v>109</v>
+        <f t="shared" ref="O90:W90" si="42">CEILING(AVERAGE(O65,O31),1)</f>
+        <v>111</v>
       </c>
       <c r="P90" s="1">
-        <f>CEILING(AVERAGE(P65,P31),1)</f>
+        <f t="shared" si="42"/>
         <v>23</v>
       </c>
       <c r="Q90" s="1">
-        <f>CEILING(AVERAGE(Q65,Q31),1)</f>
-        <v>2</v>
+        <f t="shared" si="42"/>
+        <v>3</v>
       </c>
       <c r="R90" s="1">
-        <f>CEILING(AVERAGE(R65,R31),1)</f>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="S90" s="1">
-        <f>CEILING(AVERAGE(S65,S31),1)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="T90" s="1">
-        <f>CEILING(AVERAGE(T65,T31),1)</f>
+        <f t="shared" si="42"/>
         <v>1</v>
       </c>
       <c r="U90" s="1">
-        <f>CEILING(AVERAGE(U65,U31),1)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="V90" s="1">
-        <f>CEILING(AVERAGE(V65,V31),1)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="W90" s="1">
-        <f>CEILING(AVERAGE(W65,W31),1)</f>
+        <f t="shared" si="42"/>
         <v>0</v>
       </c>
       <c r="Z90" s="1">
@@ -6132,7 +6128,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>21</v>
       </c>
@@ -6140,39 +6136,39 @@
         <v>25</v>
       </c>
       <c r="O91" s="1">
-        <f>CEILING(AVERAGE(O66,O32),1)</f>
-        <v>99</v>
+        <f t="shared" ref="O91:W91" si="43">CEILING(AVERAGE(O66,O32),1)</f>
+        <v>69</v>
       </c>
       <c r="P91" s="1">
-        <f>CEILING(AVERAGE(P66,P32),1)</f>
-        <v>16</v>
+        <f t="shared" si="43"/>
+        <v>11</v>
       </c>
       <c r="Q91" s="1">
-        <f>CEILING(AVERAGE(Q66,Q32),1)</f>
+        <f t="shared" si="43"/>
+        <v>2</v>
+      </c>
+      <c r="R91" s="1">
+        <f t="shared" si="43"/>
+        <v>1</v>
+      </c>
+      <c r="S91" s="1">
+        <f t="shared" si="43"/>
+        <v>0</v>
+      </c>
+      <c r="T91" s="1">
+        <f t="shared" si="43"/>
         <v>3</v>
       </c>
-      <c r="R91" s="1">
-        <f>CEILING(AVERAGE(R66,R32),1)</f>
-        <v>2</v>
-      </c>
-      <c r="S91" s="1">
-        <f>CEILING(AVERAGE(S66,S32),1)</f>
-        <v>1</v>
-      </c>
-      <c r="T91" s="1">
-        <f>CEILING(AVERAGE(T66,T32),1)</f>
-        <v>3</v>
-      </c>
       <c r="U91" s="1">
-        <f>CEILING(AVERAGE(U66,U32),1)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="V91" s="1">
-        <f>CEILING(AVERAGE(V66,V32),1)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="W91" s="1">
-        <f>CEILING(AVERAGE(W66,W32),1)</f>
+        <f t="shared" si="43"/>
         <v>0</v>
       </c>
       <c r="Z91" s="1">
@@ -6180,7 +6176,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>3</v>
       </c>
@@ -6188,39 +6184,39 @@
         <v>24</v>
       </c>
       <c r="O92" s="1">
-        <f>CEILING(AVERAGE(O67,O33),1)</f>
-        <v>94</v>
+        <f t="shared" ref="O92:W92" si="44">CEILING(AVERAGE(O67,O33),1)</f>
+        <v>121</v>
       </c>
       <c r="P92" s="1">
-        <f>CEILING(AVERAGE(P67,P33),1)</f>
-        <v>20</v>
+        <f t="shared" si="44"/>
+        <v>25</v>
       </c>
       <c r="Q92" s="1">
-        <f>CEILING(AVERAGE(Q67,Q33),1)</f>
-        <v>1</v>
+        <f t="shared" si="44"/>
+        <v>3</v>
       </c>
       <c r="R92" s="1">
-        <f>CEILING(AVERAGE(R67,R33),1)</f>
+        <f t="shared" si="44"/>
         <v>2</v>
       </c>
       <c r="S92" s="1">
-        <f>CEILING(AVERAGE(S67,S33),1)</f>
-        <v>0</v>
+        <f t="shared" si="44"/>
+        <v>1</v>
       </c>
       <c r="T92" s="1">
-        <f>CEILING(AVERAGE(T67,T33),1)</f>
+        <f t="shared" si="44"/>
         <v>3</v>
       </c>
       <c r="U92" s="1">
-        <f>CEILING(AVERAGE(U67,U33),1)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="V92" s="1">
-        <f>CEILING(AVERAGE(V67,V33),1)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="W92" s="1">
-        <f>CEILING(AVERAGE(W67,W33),1)</f>
+        <f t="shared" si="44"/>
         <v>0</v>
       </c>
       <c r="Z92" s="1">
@@ -6228,7 +6224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.35">
       <c r="A93" s="1" t="s">
         <v>20</v>
       </c>
@@ -6236,39 +6232,39 @@
         <v>23</v>
       </c>
       <c r="O93" s="1">
-        <f>CEILING(AVERAGE(O68,O34),1)</f>
+        <f t="shared" ref="O93:W93" si="45">CEILING(AVERAGE(O68,O34),1)</f>
         <v>70</v>
       </c>
       <c r="P93" s="1">
-        <f>CEILING(AVERAGE(P68,P34),1)</f>
+        <f t="shared" si="45"/>
         <v>11</v>
       </c>
       <c r="Q93" s="1">
-        <f>CEILING(AVERAGE(Q68,Q34),1)</f>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="R93" s="1">
-        <f>CEILING(AVERAGE(R68,R34),1)</f>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="S93" s="1">
-        <f>CEILING(AVERAGE(S68,S34),1)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="T93" s="1">
-        <f>CEILING(AVERAGE(T68,T34),1)</f>
+        <f t="shared" si="45"/>
         <v>2</v>
       </c>
       <c r="U93" s="1">
-        <f>CEILING(AVERAGE(U68,U34),1)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="V93" s="1">
-        <f>CEILING(AVERAGE(V68,V34),1)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="W93" s="1">
-        <f>CEILING(AVERAGE(W68,W34),1)</f>
+        <f t="shared" si="45"/>
         <v>0</v>
       </c>
       <c r="Z93" s="1">
@@ -6288,7 +6284,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>